<commit_message>
schema drop logic update and jarvex sql file update
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/batchsql/mysql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/batchsql/mysql_batchsql_cases.xlsx
@@ -309,18 +309,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>select p.id pid, r.id rid, r.name rname, r.`type`, r.`key`, o.code, o.name oname, r.rel_id from MYJARVEX.PERMISSION as p left join MYJARVEX.RESOURCE as r on r.id = p.RESOURCE_ID and r.parent_id = 6 left join MYJARVEX.OPERATION as o on o.id = p.OPERATION_ID where r.id in (1, 3, 6, 8, 9, 21, 22, 23, 24, 33, 34, 35, 36, 37, 38, 39, 40, 66, 67, 68)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MYJARVEX.CHAT_QU_DATA,MYJARVEX.CHAT_SE_DATA,MYJARVEX.COMMENT_BASE_INFO,MYJARVEX.CREATIVE_BASE_INFO,MYJARVEX.CREATIVE_QU_DATA,MYJARVEX.CREATIVE_SE_DATA,MYJARVEX.DATA_FILE,MYJARVEX.DATA_FILE_EXPERTISE,MYJARVEX.DATA_FILEFT,MYJARVEX.DATA_FILESET,MYJARVEX.DATA_FT_LIST,MYJARVEX.DATASET_DINGO,MYJARVEX.DATASET_FT_LIST,MYJARVEX.DEPARTMENT,MYJARVEX.MODEL_BASE_INFO,MYJARVEX.OPERATION,MYJARVEX.PERMISSION,MYJARVEX.PERMISSIONGROUP,MYJARVEX.REL_PGROUP_PERMISSION,MYJARVEX.REL_ROLE_PERMISSION,MYJARVEX.REL_ROLE_PGROUP,MYJARVEX.REL_USER_PERMISSION,MYJARVEX.REL_USER_ROLE,MYJARVEX.REL_USERGROUP_ROLE,MYJARVEX.REL_USERGROUP_USER,MYJARVEX.RESOURCE,MYJARVEX.ROLE,MYJARVEX.USER,MYJARVEX.USER_BASE,MYJARVEX.USERGROUP,MYJARVEX.VECTOR_DATA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub_component</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>MYJARVEX</t>
-  </si>
-  <si>
-    <t>select p.id pid, r.id rid, r.name rname, r.`type`, r.`key`, o.code, o.name oname, r.rel_id from MYJARVEX.PERMISSION as p left join MYJARVEX.RESOURCE as r on r.id = p.RESOURCE_ID and r.parent_id = 6 left join MYJARVEX.OPERATION as o on o.id = p.OPERATION_ID where r.id in (1, 3, 6, 8, 9, 21, 22, 23, 24, 33, 34, 35, 36, 37, 38, 39, 40, 66, 67, 68)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MYJARVEX.CHAT_QU_DATA,MYJARVEX.CHAT_SE_DATA,MYJARVEX.COMMENT_BASE_INFO,MYJARVEX.CREATIVE_BASE_INFO,MYJARVEX.CREATIVE_QU_DATA,MYJARVEX.CREATIVE_SE_DATA,MYJARVEX.DATA_FILE,MYJARVEX.DATA_FILE_EXPERTISE,MYJARVEX.DATA_FILEFT,MYJARVEX.DATA_FILESET,MYJARVEX.DATA_FT_LIST,MYJARVEX.DATASET_DINGO,MYJARVEX.DATASET_FT_LIST,MYJARVEX.DEPARTMENT,MYJARVEX.MODEL_BASE_INFO,MYJARVEX.OPERATION,MYJARVEX.PERMISSION,MYJARVEX.PERMISSIONGROUP,MYJARVEX.REL_PGROUP_PERMISSION,MYJARVEX.REL_ROLE_PERMISSION,MYJARVEX.REL_ROLE_PGROUP,MYJARVEX.REL_USER_PERMISSION,MYJARVEX.REL_USER_ROLE,MYJARVEX.REL_USERGROUP_ROLE,MYJARVEX.REL_USERGROUP_USER,MYJARVEX.RESOURCE,MYJARVEX.ROLE,MYJARVEX.USER,MYJARVEX.USER_BASE,MYJARVEX.USERGROUP,MYJARVEX.VECTOR_DATA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sub_component</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -697,7 +698,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -731,7 +732,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>82</v>
@@ -1077,17 +1078,17 @@
         <v>84</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
         <v>81</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>85</v>

</xml_diff>